<commit_message>
Pumpen und Füllkörper Recherche
</commit_message>
<xml_diff>
--- a/Arbeitsstunden recovery.xlsx
+++ b/Arbeitsstunden recovery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\E-Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC88331D-4C5A-4E72-AAE8-601816E9B3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2DB712-3E52-4AF9-A0A8-0E09C939F4E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Startzeit</t>
   </si>
@@ -144,7 +144,17 @@
     <t>Laborhandout: Beenden Bunsenbrenner und Ergänzung der restlichen Heizelemente</t>
   </si>
   <si>
-    <t>Laborhandout:</t>
+    <t>Laborhandout: Ergänzungen Heizelemente, 
+Utensilien zum Trocknen von Proben, Recherche Pumpen begonnen</t>
+  </si>
+  <si>
+    <t>Laborhandout: Recherche Laborpumpe beendet</t>
+  </si>
+  <si>
+    <t>Laborhandout: Recherche industrielle Pumpen</t>
+  </si>
+  <si>
+    <t>Laborhandout: Recherche Füllkörpertypen</t>
   </si>
 </sst>
 </file>
@@ -722,10 +732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497B6F7B-F5BE-2C40-940A-929DC888217C}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,11 +1288,11 @@
         <v>32</v>
       </c>
       <c r="F21" s="30">
-        <f t="shared" ref="F21:F27" si="5">30+$F$19-D21</f>
+        <f>30+$F$19-D21</f>
         <v>27.416666666666664</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" ref="G21:G27" si="6">120-($D$19+D21)</f>
+        <f t="shared" ref="G21:G32" si="5">120-($D$19+D21)</f>
         <v>87.416666666666657</v>
       </c>
     </row>
@@ -1297,18 +1307,18 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="D22" s="21">
-        <f t="shared" ref="D22:D28" si="7">HOUR(C22)+MINUTE(C22)/60-HOUR(B22)-MINUTE(B22)/60+D21</f>
+        <f t="shared" ref="D22:D33" si="6">HOUR(C22)+MINUTE(C22)/60-HOUR(B22)-MINUTE(B22)/60+D21</f>
         <v>3.0000000000000009</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="30">
+        <f>30+$F$19-D22</f>
+        <v>26.416666666666664</v>
+      </c>
+      <c r="G22" s="9">
         <f t="shared" si="5"/>
-        <v>26.416666666666664</v>
-      </c>
-      <c r="G22" s="9">
-        <f t="shared" si="6"/>
         <v>86.416666666666657</v>
       </c>
     </row>
@@ -1323,18 +1333,18 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D23" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>7.0000000000000009</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="30">
+        <f t="shared" ref="F23:F32" si="7">30+$F$19-D23</f>
+        <v>22.416666666666664</v>
+      </c>
+      <c r="G23" s="9">
         <f t="shared" si="5"/>
-        <v>22.416666666666664</v>
-      </c>
-      <c r="G23" s="9">
-        <f t="shared" si="6"/>
         <v>82.416666666666657</v>
       </c>
     </row>
@@ -1349,18 +1359,18 @@
         <v>0.5625</v>
       </c>
       <c r="D24" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>8.75</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="30">
+        <f t="shared" si="7"/>
+        <v>20.666666666666664</v>
+      </c>
+      <c r="G24" s="9">
         <f t="shared" si="5"/>
-        <v>20.666666666666664</v>
-      </c>
-      <c r="G24" s="9">
-        <f t="shared" si="6"/>
         <v>80.666666666666657</v>
       </c>
     </row>
@@ -1375,18 +1385,18 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="D25" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>11.25</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F25" s="30">
+        <f t="shared" si="7"/>
+        <v>18.166666666666664</v>
+      </c>
+      <c r="G25" s="9">
         <f t="shared" si="5"/>
-        <v>18.166666666666664</v>
-      </c>
-      <c r="G25" s="9">
-        <f t="shared" si="6"/>
         <v>78.166666666666657</v>
       </c>
     </row>
@@ -1401,22 +1411,22 @@
         <v>0.375</v>
       </c>
       <c r="D26" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>12.25</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>35</v>
       </c>
       <c r="F26" s="30">
+        <f t="shared" si="7"/>
+        <v>17.166666666666664</v>
+      </c>
+      <c r="G26" s="9">
         <f t="shared" si="5"/>
-        <v>17.166666666666664</v>
-      </c>
-      <c r="G26" s="9">
-        <f t="shared" si="6"/>
         <v>77.166666666666657</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>44186</v>
       </c>
@@ -1424,67 +1434,161 @@
         <v>0.5625</v>
       </c>
       <c r="C27" s="7">
-        <v>0.6875</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="D27" s="21">
+        <f t="shared" si="6"/>
+        <v>15.333333333333332</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="30">
         <f t="shared" si="7"/>
-        <v>15.25</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="30">
+        <v>14.083333333333332</v>
+      </c>
+      <c r="G27" s="9">
         <f t="shared" si="5"/>
-        <v>14.166666666666664</v>
-      </c>
-      <c r="G27" s="9">
-        <f t="shared" si="6"/>
-        <v>74.166666666666657</v>
+        <v>74.083333333333329</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
-        <v>44193</v>
+        <v>44187</v>
       </c>
       <c r="B28" s="7">
-        <v>0.375</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C28" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="D28" s="21">
-        <f>HOUR(C28)+MINUTE(C28)/60-HOUR(B28)-MINUTE(B28)/60+D27</f>
-        <v>20.25</v>
+        <f t="shared" si="6"/>
+        <v>16.75</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="30">
+        <f t="shared" si="7"/>
+        <v>12.666666666666664</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="5"/>
+        <v>72.666666666666657</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
-        <v>44194</v>
+        <v>44187</v>
       </c>
       <c r="B29" s="7">
-        <v>0.375</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="C29" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="D29" s="21">
-        <f t="shared" ref="D29:D30" si="8">HOUR(C29)+MINUTE(C29)/60-HOUR(B29)-MINUTE(B29)/60+D28</f>
-        <v>25.25</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="30">
+        <f t="shared" si="7"/>
+        <v>11.416666666666664</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="5"/>
+        <v>71.416666666666657</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
+        <v>44187</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D30" s="21">
+        <f t="shared" si="6"/>
+        <v>18.166666666666668</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="30">
+        <f t="shared" si="7"/>
+        <v>11.249999999999996</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="5"/>
+        <v>71.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <v>44193</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D31" s="21">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F31" s="30">
+        <f t="shared" si="7"/>
+        <v>9.4166666666666643</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="5"/>
+        <v>69.416666666666657</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <v>44194</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D32" s="21">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="F32" s="30">
+        <f t="shared" si="7"/>
+        <v>4.4166666666666643</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="5"/>
+        <v>64.416666666666657</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
         <v>44195</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B33" s="7">
         <v>0.375</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C33" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D30" s="21">
-        <f t="shared" si="8"/>
-        <v>30.25</v>
+      <c r="D33" s="21">
+        <f t="shared" si="6"/>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3d Modelle und Überarbeitung
</commit_message>
<xml_diff>
--- a/Arbeitsstunden recovery.xlsx
+++ b/Arbeitsstunden recovery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\E-Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CACF8-E5AD-450B-A3B1-792D85C76CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B86FD8B-9C22-46B6-850E-3A04A2EC5E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Startzeit</t>
   </si>
@@ -158,6 +158,19 @@
   </si>
   <si>
     <t>Laborhandout: Beginn des Übertragens der recherschierten Pumpen Infos in Dokument</t>
+  </si>
+  <si>
+    <t>Labborhandout: Pumpenübersicht, Füllkörper, Beschriftung mit Edding</t>
+  </si>
+  <si>
+    <t>Laborhandout: Normschliffe, Schlifffett, Eismaschine, Ultraschallbad</t>
+  </si>
+  <si>
+    <t>Laborhandout: Überarbeitung - 3D-Modell Muffe mit Erklärung</t>
+  </si>
+  <si>
+    <t>Laborhandout: Überarbeitung Layout +  Formulierung, 
+Recherche und Erstellung von 3D Modellen für Rührer</t>
   </si>
 </sst>
 </file>
@@ -735,10 +748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497B6F7B-F5BE-2C40-940A-929DC888217C}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,22 +1268,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C20" s="7">
-        <v>0.50347222222222221</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="D20" s="21">
         <f>HOUR(C20)+MINUTE(C20)/60-HOUR(B20)-MINUTE(B20)/60</f>
-        <v>0.75000000000000067</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="30">
         <f>30+$F$19-D20</f>
-        <v>28.666666666666664</v>
+        <v>28.499999999999996</v>
       </c>
       <c r="G20" s="9">
         <f>120-($D$19+D20)</f>
-        <v>88.666666666666657</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1281,22 +1294,22 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C21" s="7">
-        <v>0.59375</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D21" s="21">
         <f>HOUR(C21)+MINUTE(C21)/60-HOUR(B21)-MINUTE(B21)/60+D20</f>
-        <v>2.0000000000000009</v>
+        <v>2.416666666666667</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>32</v>
       </c>
       <c r="F21" s="30">
         <f>30+$F$19-D21</f>
-        <v>27.416666666666664</v>
+        <v>26.999999999999996</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" ref="G21:G33" si="5">120-($D$19+D21)</f>
-        <v>87.416666666666657</v>
+        <f t="shared" ref="G21:G35" si="5">120-($D$19+D21)</f>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,22 +1320,22 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="C22" s="7">
-        <v>0.73958333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="D22" s="21">
-        <f t="shared" ref="D22:D33" si="6">HOUR(C22)+MINUTE(C22)/60-HOUR(B22)-MINUTE(B22)/60+D21</f>
-        <v>3.0000000000000009</v>
+        <f t="shared" ref="D22:D35" si="6">HOUR(C22)+MINUTE(C22)/60-HOUR(B22)-MINUTE(B22)/60+D21</f>
+        <v>3.666666666666667</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="30">
         <f>30+$F$19-D22</f>
-        <v>26.416666666666664</v>
+        <v>25.749999999999996</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="5"/>
-        <v>86.416666666666657</v>
+        <v>85.75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,22 +1346,22 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C23" s="7">
-        <v>0.70833333333333337</v>
+        <v>0.71875</v>
       </c>
       <c r="D23" s="21">
         <f t="shared" si="6"/>
-        <v>7.0000000000000009</v>
+        <v>7.916666666666667</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="30">
         <f t="shared" ref="F23:F31" si="7">30+$F$19-D23</f>
-        <v>22.416666666666664</v>
+        <v>21.499999999999996</v>
       </c>
       <c r="G23" s="9">
         <f t="shared" si="5"/>
-        <v>82.416666666666657</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,22 +1372,22 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="C24" s="7">
-        <v>0.5625</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D24" s="21">
         <f t="shared" si="6"/>
-        <v>8.75</v>
+        <v>9.9166666666666679</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="30">
         <f t="shared" si="7"/>
-        <v>20.666666666666664</v>
+        <v>19.499999999999996</v>
       </c>
       <c r="G24" s="9">
         <f t="shared" si="5"/>
-        <v>80.666666666666657</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,22 +1398,22 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="C25" s="7">
-        <v>0.67708333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="D25" s="21">
         <f t="shared" si="6"/>
-        <v>11.25</v>
+        <v>12.666666666666668</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F25" s="30">
-        <f t="shared" si="7"/>
-        <v>18.166666666666664</v>
+        <f>30+$F$19-D25</f>
+        <v>16.749999999999996</v>
       </c>
       <c r="G25" s="9">
         <f t="shared" si="5"/>
-        <v>78.166666666666657</v>
+        <v>76.75</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,22 +1424,22 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C26" s="7">
-        <v>0.375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="D26" s="21">
         <f t="shared" si="6"/>
-        <v>12.25</v>
+        <v>13.916666666666668</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>35</v>
       </c>
       <c r="F26" s="30">
         <f t="shared" si="7"/>
-        <v>17.166666666666664</v>
+        <v>15.499999999999996</v>
       </c>
       <c r="G26" s="9">
         <f t="shared" si="5"/>
-        <v>77.166666666666657</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1437,22 +1450,22 @@
         <v>0.5625</v>
       </c>
       <c r="C27" s="7">
-        <v>0.69097222222222221</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="D27" s="21">
         <f t="shared" si="6"/>
-        <v>15.333333333333332</v>
+        <v>17.25</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F27" s="30">
-        <f t="shared" si="7"/>
-        <v>14.083333333333332</v>
+        <f>30+$F$19-D27</f>
+        <v>12.166666666666664</v>
       </c>
       <c r="G27" s="9">
         <f t="shared" si="5"/>
-        <v>74.083333333333329</v>
+        <v>72.166666666666657</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1463,22 +1476,22 @@
         <v>0.3888888888888889</v>
       </c>
       <c r="C28" s="7">
-        <v>0.44791666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D28" s="21">
         <f t="shared" si="6"/>
-        <v>16.75</v>
+        <v>18.916666666666668</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>37</v>
       </c>
       <c r="F28" s="30">
         <f t="shared" si="7"/>
-        <v>12.666666666666664</v>
+        <v>10.499999999999996</v>
       </c>
       <c r="G28" s="9">
         <f t="shared" si="5"/>
-        <v>72.666666666666657</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1489,22 +1502,22 @@
         <v>0.46180555555555558</v>
       </c>
       <c r="C29" s="7">
-        <v>0.51388888888888895</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="D29" s="21">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>20.416666666666668</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="30">
-        <f t="shared" si="7"/>
-        <v>11.416666666666664</v>
+        <f>30+$F$19-D29</f>
+        <v>8.9999999999999964</v>
       </c>
       <c r="G29" s="9">
         <f t="shared" si="5"/>
-        <v>71.416666666666657</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1515,94 +1528,152 @@
         <v>0.51388888888888895</v>
       </c>
       <c r="C30" s="7">
-        <v>0.52083333333333337</v>
+        <v>0.53125</v>
       </c>
       <c r="D30" s="21">
         <f t="shared" si="6"/>
-        <v>18.166666666666668</v>
+        <v>20.833333333333336</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F30" s="30">
         <f t="shared" si="7"/>
-        <v>11.249999999999996</v>
+        <v>8.5833333333333286</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="5"/>
-        <v>71.25</v>
+        <v>68.583333333333329</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
-        <v>44193</v>
+        <v>44187</v>
       </c>
       <c r="B31" s="7">
         <v>0.62847222222222221</v>
       </c>
       <c r="C31" s="7">
-        <v>0.6875</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D31" s="21">
         <f t="shared" si="6"/>
-        <v>19.583333333333336</v>
+        <v>22.500000000000004</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="30">
         <f t="shared" si="7"/>
-        <v>9.8333333333333286</v>
+        <v>6.9166666666666607</v>
       </c>
       <c r="G31" s="9">
         <f t="shared" si="5"/>
-        <v>69.833333333333329</v>
+        <v>66.916666666666657</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
-        <v>44194</v>
+        <v>44192</v>
       </c>
       <c r="B32" s="7">
-        <v>0.375</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C32" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="D32" s="21">
         <f t="shared" si="6"/>
-        <v>24.583333333333336</v>
+        <v>24.250000000000004</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="F32" s="30">
         <f>30+$F$19-D32</f>
-        <v>4.8333333333333286</v>
+        <v>5.1666666666666607</v>
       </c>
       <c r="G32" s="9">
         <f t="shared" si="5"/>
-        <v>64.833333333333329</v>
+        <v>65.166666666666657</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
-        <v>44195</v>
+        <v>44192</v>
       </c>
       <c r="B33" s="7">
-        <v>0.375</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="C33" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.65625</v>
       </c>
       <c r="D33" s="21">
         <f t="shared" si="6"/>
-        <v>29.583333333333336</v>
+        <v>25.250000000000004</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F33" s="30">
         <f>30+$F$19-D33</f>
-        <v>-0.1666666666666714</v>
+        <v>4.1666666666666607</v>
       </c>
       <c r="G33" s="9">
         <f t="shared" si="5"/>
-        <v>59.833333333333329</v>
+        <v>64.166666666666657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <v>43832</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D34" s="21">
+        <f t="shared" si="6"/>
+        <v>27.750000000000004</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="30">
+        <f>30+$F$19-D34</f>
+        <v>1.6666666666666607</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="5"/>
+        <v>61.666666666666657</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>43832</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D35" s="21">
+        <f t="shared" si="6"/>
+        <v>31.000000000000004</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="30">
+        <f>30+$F$19-D35</f>
+        <v>-1.5833333333333393</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="5"/>
+        <v>58.416666666666657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>